<commit_message>
completar para creacion de tabla pivote
</commit_message>
<xml_diff>
--- a/mapeo PU.xlsx
+++ b/mapeo PU.xlsx
@@ -983,9 +983,6 @@
     </r>
   </si>
   <si>
-    <t>consultar a Fico</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Corresponde al clasificador 109, fk a la tabla </t>
     </r>
@@ -1003,6 +1000,21 @@
   <si>
     <r>
       <t xml:space="preserve">Corresponde al clasificador 110, fk a la tabla </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Clasificador.DetalleClasificador</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Corresponde al clasificador 111, fk a la tabla </t>
     </r>
     <r>
       <rPr>
@@ -1135,19 +1147,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1159,10 +1171,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1445,8 +1461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1499,12 +1515,13 @@
       <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="3" t="s">
         <v>122</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
@@ -1514,12 +1531,13 @@
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="3" t="s">
         <v>80</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
@@ -1529,12 +1547,13 @@
       <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
@@ -1550,6 +1569,7 @@
       <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
@@ -1559,12 +1579,13 @@
       <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="3" t="s">
         <v>76</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
@@ -1574,12 +1595,13 @@
       <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="3" t="s">
         <v>77</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
@@ -1595,6 +1617,7 @@
       <c r="E9" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
@@ -1604,15 +1627,13 @@
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="3" t="s">
         <v>79</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>124</v>
-      </c>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
@@ -1622,10 +1643,11 @@
       <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="3" t="s">
         <v>82</v>
       </c>
       <c r="E11" s="2"/>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
@@ -1635,13 +1657,14 @@
       <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="3" t="s">
         <v>123</v>
       </c>
       <c r="E12" s="2"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1650,45 +1673,48 @@
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="3" t="s">
         <v>97</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="3" t="s">
         <v>122</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="3" t="s">
         <v>122</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
@@ -1701,9 +1727,10 @@
       <c r="E16" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
       <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1716,9 +1743,10 @@
       <c r="E17" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1731,9 +1759,10 @@
       <c r="E18" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
       <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
@@ -1746,9 +1775,10 @@
       <c r="E19" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1761,9 +1791,10 @@
       <c r="E20" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
       <c r="B21" s="2" t="s">
         <v>28</v>
       </c>
@@ -1776,9 +1807,10 @@
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
       <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
@@ -1791,9 +1823,10 @@
       <c r="E22" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
       <c r="B23" s="2" t="s">
         <v>30</v>
       </c>
@@ -1804,9 +1837,10 @@
       <c r="E23" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
       <c r="B24" s="2" t="s">
         <v>8</v>
       </c>
@@ -1819,9 +1853,10 @@
       <c r="E24" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
       <c r="B25" s="2" t="s">
         <v>31</v>
       </c>
@@ -1834,9 +1869,10 @@
       <c r="E25" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
       <c r="B26" s="2" t="s">
         <v>32</v>
       </c>
@@ -1847,9 +1883,10 @@
       <c r="E26" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="F26" s="10"/>
+    </row>
+    <row r="27" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1858,30 +1895,32 @@
       <c r="C27" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="3" t="s">
         <v>80</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
+      <c r="F27" s="10"/>
+    </row>
+    <row r="28" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
       <c r="B28" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
+      <c r="F28" s="10"/>
+    </row>
+    <row r="29" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
       <c r="B29" s="2" t="s">
         <v>37</v>
       </c>
@@ -1894,245 +1933,262 @@
       <c r="E29" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
       <c r="B30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="3" t="s">
         <v>122</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
+      <c r="F30" s="10"/>
+    </row>
+    <row r="31" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A31" s="5"/>
       <c r="B31" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="3" t="s">
         <v>85</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
+      <c r="F31" s="10"/>
+    </row>
+    <row r="32" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A32" s="5"/>
       <c r="B32" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
+      <c r="F32" s="10"/>
+    </row>
+    <row r="33" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A33" s="5"/>
       <c r="B33" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="3" t="s">
         <v>87</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
+      <c r="F33" s="10"/>
+    </row>
+    <row r="34" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A34" s="5"/>
       <c r="B34" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="3" t="s">
         <v>88</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+      <c r="F34" s="10"/>
+    </row>
+    <row r="35" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A35" s="5"/>
       <c r="B35" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="3" t="s">
         <v>89</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A36" s="5"/>
       <c r="B36" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="3" t="s">
         <v>79</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A37" s="5"/>
       <c r="B37" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="3" t="s">
         <v>90</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="4"/>
+      <c r="F37" s="10"/>
+    </row>
+    <row r="38" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A38" s="5"/>
       <c r="B38" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D38" s="3" t="s">
         <v>91</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A39" s="4"/>
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A39" s="5"/>
       <c r="B39" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D39" s="3" t="s">
         <v>92</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A40" s="4"/>
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A40" s="5"/>
       <c r="B40" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="3" t="s">
         <v>93</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A41" s="4"/>
+      <c r="F40" s="10"/>
+    </row>
+    <row r="41" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A41" s="5"/>
       <c r="B41" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D41" s="3" t="s">
         <v>94</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
+      <c r="F41" s="10"/>
+    </row>
+    <row r="42" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A42" s="5"/>
       <c r="B42" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D42" s="3" t="s">
         <v>95</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
+      <c r="F42" s="10"/>
+    </row>
+    <row r="43" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A43" s="5"/>
       <c r="B43" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D43" s="3" t="s">
         <v>96</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A44" s="4"/>
+      <c r="F43" s="10"/>
+    </row>
+    <row r="44" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A44" s="5"/>
       <c r="B44" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D44" s="9"/>
+      <c r="D44" s="3"/>
       <c r="E44" s="2"/>
-    </row>
-    <row r="45" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A45" s="4"/>
+      <c r="F44" s="10"/>
+    </row>
+    <row r="45" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A45" s="5"/>
       <c r="B45" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D45" s="3" t="s">
         <v>84</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
+      <c r="F45" s="10"/>
+    </row>
+    <row r="46" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -2141,30 +2197,32 @@
       <c r="C46" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D46" s="3" t="s">
         <v>122</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A47" s="4"/>
+      <c r="F46" s="10"/>
+    </row>
+    <row r="47" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A47" s="5"/>
       <c r="B47" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D47" s="9" t="s">
+      <c r="D47" s="3" t="s">
         <v>122</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A48" s="4"/>
+      <c r="F47" s="10"/>
+    </row>
+    <row r="48" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A48" s="5"/>
       <c r="B48" s="2" t="s">
         <v>49</v>
       </c>
@@ -2177,54 +2235,58 @@
       <c r="E48" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A49" s="4"/>
+      <c r="F48" s="10"/>
+    </row>
+    <row r="49" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A49" s="5"/>
       <c r="B49" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D49" s="9" t="s">
+      <c r="D49" s="3" t="s">
         <v>80</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A50" s="4"/>
+      <c r="F49" s="10"/>
+    </row>
+    <row r="50" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A50" s="5"/>
       <c r="B50" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D50" s="9" t="s">
+      <c r="D50" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A51" s="4"/>
+      <c r="F50" s="10"/>
+    </row>
+    <row r="51" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A51" s="5"/>
       <c r="B51" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D51" s="9" t="s">
-        <v>126</v>
+      <c r="D51" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A52" s="4"/>
+      <c r="F51" s="10"/>
+    </row>
+    <row r="52" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A52" s="5"/>
       <c r="B52" s="2" t="s">
         <v>51</v>
       </c>
@@ -2237,52 +2299,58 @@
       <c r="E52" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A53" s="4"/>
+      <c r="F52" s="10"/>
+    </row>
+    <row r="53" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A53" s="5"/>
       <c r="B53" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D53" s="2"/>
+      <c r="D53" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E53" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A54" s="4"/>
+      <c r="F53" s="10"/>
+    </row>
+    <row r="54" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A54" s="5"/>
       <c r="B54" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D54" s="9" t="s">
+      <c r="D54" s="3" t="s">
         <v>100</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A55" s="5"/>
+      <c r="F54" s="10"/>
+    </row>
+    <row r="55" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A55" s="9"/>
       <c r="B55" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D55" s="9" t="s">
-        <v>125</v>
+      <c r="D55" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A56" s="3" t="s">
+      <c r="F55" s="10"/>
+    </row>
+    <row r="56" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
         <v>63</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -2291,15 +2359,16 @@
       <c r="C56" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D56" s="9" t="s">
+      <c r="D56" s="3" t="s">
         <v>122</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A57" s="4"/>
+      <c r="F56" s="10"/>
+    </row>
+    <row r="57" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A57" s="5"/>
       <c r="B57" s="2" t="s">
         <v>49</v>
       </c>
@@ -2312,39 +2381,42 @@
       <c r="E57" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A58" s="4"/>
+      <c r="F57" s="10"/>
+    </row>
+    <row r="58" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A58" s="5"/>
       <c r="B58" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D58" s="9" t="s">
+      <c r="D58" s="3" t="s">
         <v>80</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A59" s="4"/>
+      <c r="F58" s="10"/>
+    </row>
+    <row r="59" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A59" s="5"/>
       <c r="B59" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D59" s="9" t="s">
+      <c r="D59" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A60" s="4"/>
+      <c r="F59" s="10"/>
+    </row>
+    <row r="60" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A60" s="5"/>
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
@@ -2357,24 +2429,26 @@
       <c r="E60" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A61" s="4"/>
+      <c r="F60" s="10"/>
+    </row>
+    <row r="61" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A61" s="5"/>
       <c r="B61" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D61" s="9" t="s">
+      <c r="D61" s="3" t="s">
         <v>79</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A62" s="4"/>
+      <c r="F61" s="10"/>
+    </row>
+    <row r="62" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A62" s="5"/>
       <c r="B62" s="2" t="s">
         <v>55</v>
       </c>
@@ -2387,9 +2461,10 @@
       <c r="E62" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A63" s="4"/>
+      <c r="F62" s="10"/>
+    </row>
+    <row r="63" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A63" s="5"/>
       <c r="B63" s="2" t="s">
         <v>56</v>
       </c>
@@ -2402,9 +2477,10 @@
       <c r="E63" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A64" s="4"/>
+      <c r="F63" s="10"/>
+    </row>
+    <row r="64" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A64" s="5"/>
       <c r="B64" s="2" t="s">
         <v>57</v>
       </c>
@@ -2417,9 +2493,10 @@
       <c r="E64" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A65" s="4"/>
+      <c r="F64" s="10"/>
+    </row>
+    <row r="65" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A65" s="5"/>
       <c r="B65" s="2" t="s">
         <v>58</v>
       </c>
@@ -2432,9 +2509,10 @@
       <c r="E65" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A66" s="4"/>
+      <c r="F65" s="10"/>
+    </row>
+    <row r="66" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A66" s="5"/>
       <c r="B66" s="2" t="s">
         <v>59</v>
       </c>
@@ -2447,9 +2525,10 @@
       <c r="E66" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A67" s="4"/>
+      <c r="F66" s="10"/>
+    </row>
+    <row r="67" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A67" s="5"/>
       <c r="B67" s="2" t="s">
         <v>60</v>
       </c>
@@ -2462,9 +2541,10 @@
       <c r="E67" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A68" s="4"/>
+      <c r="F67" s="10"/>
+    </row>
+    <row r="68" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A68" s="5"/>
       <c r="B68" s="2" t="s">
         <v>61</v>
       </c>
@@ -2477,9 +2557,10 @@
       <c r="E68" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A69" s="4"/>
+      <c r="F68" s="10"/>
+    </row>
+    <row r="69" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A69" s="5"/>
       <c r="B69" s="2" t="s">
         <v>62</v>
       </c>
@@ -2492,24 +2573,26 @@
       <c r="E69" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A70" s="4"/>
+      <c r="F69" s="10"/>
+    </row>
+    <row r="70" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A70" s="5"/>
       <c r="B70" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D70" s="9" t="s">
-        <v>125</v>
+      <c r="D70" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A71" s="3" t="s">
+      <c r="F70" s="10"/>
+    </row>
+    <row r="71" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A71" s="12" t="s">
         <v>67</v>
       </c>
       <c r="B71" s="2" t="s">
@@ -2518,45 +2601,48 @@
       <c r="C71" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D71" s="9" t="s">
+      <c r="D71" s="3" t="s">
         <v>122</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A72" s="4"/>
+      <c r="F71" s="10"/>
+    </row>
+    <row r="72" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A72" s="12"/>
       <c r="B72" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D72" s="9" t="s">
+      <c r="D72" s="3" t="s">
         <v>80</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A73" s="4"/>
+      <c r="F72" s="10"/>
+    </row>
+    <row r="73" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A73" s="12"/>
       <c r="B73" s="2" t="s">
         <v>70</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D73" s="9" t="s">
+      <c r="D73" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A74" s="4"/>
+      <c r="F73" s="10"/>
+    </row>
+    <row r="74" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A74" s="12"/>
       <c r="B74" s="2" t="s">
         <v>6</v>
       </c>
@@ -2569,9 +2655,10 @@
       <c r="E74" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A75" s="4"/>
+      <c r="F74" s="10"/>
+    </row>
+    <row r="75" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A75" s="12"/>
       <c r="B75" s="2" t="s">
         <v>49</v>
       </c>
@@ -2584,9 +2671,10 @@
       <c r="E75" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A76" s="4"/>
+      <c r="F75" s="10"/>
+    </row>
+    <row r="76" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A76" s="12"/>
       <c r="B76" s="2" t="s">
         <v>55</v>
       </c>
@@ -2599,9 +2687,10 @@
       <c r="E76" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A77" s="4"/>
+      <c r="F76" s="10"/>
+    </row>
+    <row r="77" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A77" s="12"/>
       <c r="B77" s="2" t="s">
         <v>65</v>
       </c>
@@ -2614,9 +2703,10 @@
       <c r="E77" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A78" s="4"/>
+      <c r="F77" s="10"/>
+    </row>
+    <row r="78" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A78" s="12"/>
       <c r="B78" s="2" t="s">
         <v>66</v>
       </c>
@@ -2629,21 +2719,23 @@
       <c r="E78" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="A79" s="4"/>
+      <c r="F78" s="10"/>
+    </row>
+    <row r="79" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A79" s="12"/>
       <c r="B79" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D79" s="9" t="s">
-        <v>125</v>
+      <c r="D79" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="F79" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
migracion pu con tablas pivote
</commit_message>
<xml_diff>
--- a/mapeo PU.xlsx
+++ b/mapeo PU.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="127">
   <si>
     <t>Mapeo de datos origen y destino - PAGO UNICO</t>
   </si>
@@ -570,7 +570,37 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Corresponde al clasificador (a ser creado), fk a la tabla </t>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>PORCENTAJE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>FORMULARIO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Corresponde al clasificador 2, fk a la tabla </t>
     </r>
     <r>
       <rPr>
@@ -595,7 +625,7 @@
         <rFont val="Arial Narrow"/>
         <family val="2"/>
       </rPr>
-      <t>PORCENTAJE</t>
+      <t>NUM_CERTIF</t>
     </r>
   </si>
   <si>
@@ -610,12 +640,321 @@
         <rFont val="Arial Narrow"/>
         <family val="2"/>
       </rPr>
-      <t>FORMULARIO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Corresponde al clasificador 2, fk a la tabla </t>
+      <t>ANIOS_INSALUBRES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>MONTO_BASE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>REINTEGRO_DESDE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>REINTEGRO_HASTA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>REINTEGRO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>AGUINALDO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>RED_EDAD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>MESES_CNS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>NUM_CERTIF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>FECHA_ALTA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>RESOLUCION</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>COD</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>ANIO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>MES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>DEBE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>HABER</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>NRO_CHEQUE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>NRO_BAN</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>FECHA_EMI</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dato propio de la tabla, campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>C31</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Corresponde al identificador de la persona, fk a la tabla </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>Persona.Persona</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Corresponde al clasificador 106: Pago Unico, fk a la tabla </t>
     </r>
     <r>
       <rPr>
@@ -630,346 +969,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>NUM_CERTIF</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>ANIOS_INSALUBRES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>MONTO_BASE</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>REINTEGRO_DESDE</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>REINTEGRO_HASTA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>REINTEGRO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>AGUINALDO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>RED_EDAD</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>MESES_CNS</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>NUM_CERTIF</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>FECHA_ALTA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>RESOLUCION</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>COD</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>ANIO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>MES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>DEBE</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>HABER</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>NRO_CHEQUE</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>NRO_BAN</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>FECHA_EMI</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Dato propio de la tabla, campo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>C31</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Corresponde al identificador de la persona, fk a la tabla </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>Persona.Persona</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Corresponde al clasificador 106: Pago Unico, fk a la tabla </t>
+      <t xml:space="preserve">Corresponde al clasificador 109, fk a la tabla </t>
     </r>
     <r>
       <rPr>
@@ -984,7 +984,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Corresponde al clasificador 109, fk a la tabla </t>
+      <t xml:space="preserve">Corresponde al clasificador 110, fk a la tabla </t>
     </r>
     <r>
       <rPr>
@@ -999,7 +999,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Corresponde al clasificador 110, fk a la tabla </t>
+      <t xml:space="preserve">Corresponde al clasificador 111, fk a la tabla </t>
     </r>
     <r>
       <rPr>
@@ -1014,7 +1014,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Corresponde al clasificador 111, fk a la tabla </t>
+      <t xml:space="preserve">Corresponde al clasificador 93, fk a la tabla </t>
     </r>
     <r>
       <rPr>
@@ -1156,10 +1156,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1171,12 +1170,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1461,8 +1461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,14 +1476,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1506,7 +1506,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1516,15 +1516,15 @@
         <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="10"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="2" t="s">
         <v>69</v>
       </c>
@@ -1537,10 +1537,10 @@
       <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="10"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="2" t="s">
         <v>70</v>
       </c>
@@ -1553,10 +1553,10 @@
       <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="10"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1569,10 +1569,10 @@
       <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1585,10 +1585,10 @@
       <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1601,10 +1601,10 @@
       <c r="E8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="10"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1617,10 +1617,10 @@
       <c r="E9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="10"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1633,10 +1633,10 @@
       <c r="E10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="11"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1647,10 +1647,10 @@
         <v>82</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="10"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1658,13 +1658,13 @@
         <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="10"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1674,15 +1674,15 @@
         <v>19</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="10"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
@@ -1690,15 +1690,15 @@
         <v>13</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="10"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
@@ -1706,15 +1706,15 @@
         <v>13</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="10"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
@@ -1722,15 +1722,15 @@
         <v>33</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="10"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1738,15 +1738,15 @@
         <v>19</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="10"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
@@ -1754,15 +1754,15 @@
         <v>34</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="10"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
@@ -1770,15 +1770,15 @@
         <v>35</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="10"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1786,15 +1786,15 @@
         <v>35</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="10"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="2" t="s">
         <v>28</v>
       </c>
@@ -1802,15 +1802,15 @@
         <v>19</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="10"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
+      <c r="A22" s="11"/>
       <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
@@ -1818,29 +1818,31 @@
         <v>19</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="10"/>
-    </row>
-    <row r="23" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
       <c r="B23" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="10"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="2" t="s">
         <v>8</v>
       </c>
@@ -1848,15 +1850,15 @@
         <v>16</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="10"/>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
+      <c r="A25" s="11"/>
       <c r="B25" s="2" t="s">
         <v>31</v>
       </c>
@@ -1864,15 +1866,15 @@
         <v>19</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F25" s="10"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="2" t="s">
         <v>32</v>
       </c>
@@ -1883,10 +1885,10 @@
       <c r="E26" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="10"/>
+      <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1901,10 +1903,10 @@
       <c r="E27" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="10"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
+      <c r="A28" s="11"/>
       <c r="B28" s="2" t="s">
         <v>70</v>
       </c>
@@ -1917,10 +1919,10 @@
       <c r="E28" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F28" s="10"/>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="2" t="s">
         <v>37</v>
       </c>
@@ -1933,10 +1935,10 @@
       <c r="E29" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F29" s="10"/>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="2" t="s">
         <v>5</v>
       </c>
@@ -1944,15 +1946,15 @@
         <v>13</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F30" s="10"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
+      <c r="A31" s="11"/>
       <c r="B31" s="2" t="s">
         <v>38</v>
       </c>
@@ -1965,10 +1967,10 @@
       <c r="E31" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F31" s="10"/>
+      <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="2" t="s">
         <v>39</v>
       </c>
@@ -1981,10 +1983,10 @@
       <c r="E32" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="10"/>
+      <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="2" t="s">
         <v>71</v>
       </c>
@@ -1997,10 +1999,10 @@
       <c r="E33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F33" s="10"/>
+      <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="2" t="s">
         <v>40</v>
       </c>
@@ -2013,10 +2015,10 @@
       <c r="E34" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F34" s="10"/>
+      <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A35" s="5"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="2" t="s">
         <v>41</v>
       </c>
@@ -2029,10 +2031,10 @@
       <c r="E35" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F35" s="10"/>
+      <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="2" t="s">
         <v>10</v>
       </c>
@@ -2045,10 +2047,10 @@
       <c r="E36" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F36" s="10"/>
+      <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="2" t="s">
         <v>42</v>
       </c>
@@ -2061,10 +2063,10 @@
       <c r="E37" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F37" s="10"/>
+      <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="5"/>
+      <c r="A38" s="11"/>
       <c r="B38" s="2" t="s">
         <v>43</v>
       </c>
@@ -2077,10 +2079,10 @@
       <c r="E38" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="10"/>
+      <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
+      <c r="A39" s="11"/>
       <c r="B39" s="2" t="s">
         <v>44</v>
       </c>
@@ -2093,10 +2095,10 @@
       <c r="E39" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F39" s="10"/>
+      <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
+      <c r="A40" s="11"/>
       <c r="B40" s="2" t="s">
         <v>45</v>
       </c>
@@ -2109,10 +2111,10 @@
       <c r="E40" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F40" s="10"/>
+      <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A41" s="5"/>
+      <c r="A41" s="11"/>
       <c r="B41" s="2" t="s">
         <v>46</v>
       </c>
@@ -2125,10 +2127,10 @@
       <c r="E41" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F41" s="10"/>
+      <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
+      <c r="A42" s="11"/>
       <c r="B42" s="2" t="s">
         <v>47</v>
       </c>
@@ -2141,10 +2143,10 @@
       <c r="E42" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F42" s="10"/>
+      <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A43" s="5"/>
+      <c r="A43" s="11"/>
       <c r="B43" s="2" t="s">
         <v>72</v>
       </c>
@@ -2157,10 +2159,10 @@
       <c r="E43" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F43" s="10"/>
+      <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A44" s="5"/>
+      <c r="A44" s="11"/>
       <c r="B44" s="2" t="s">
         <v>73</v>
       </c>
@@ -2169,10 +2171,10 @@
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="2"/>
-      <c r="F44" s="10"/>
+      <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A45" s="5"/>
+      <c r="A45" s="11"/>
       <c r="B45" s="2" t="s">
         <v>12</v>
       </c>
@@ -2185,10 +2187,10 @@
       <c r="E45" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F45" s="10"/>
+      <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="10" t="s">
         <v>54</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -2198,15 +2200,15 @@
         <v>13</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F46" s="10"/>
+      <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A47" s="5"/>
+      <c r="A47" s="11"/>
       <c r="B47" s="2" t="s">
         <v>25</v>
       </c>
@@ -2214,15 +2216,15 @@
         <v>13</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F47" s="10"/>
+      <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A48" s="5"/>
+      <c r="A48" s="11"/>
       <c r="B48" s="2" t="s">
         <v>49</v>
       </c>
@@ -2230,15 +2232,15 @@
         <v>19</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F48" s="10"/>
+      <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A49" s="5"/>
+      <c r="A49" s="11"/>
       <c r="B49" s="2" t="s">
         <v>69</v>
       </c>
@@ -2251,10 +2253,10 @@
       <c r="E49" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F49" s="10"/>
+      <c r="F49" s="4"/>
     </row>
     <row r="50" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A50" s="5"/>
+      <c r="A50" s="11"/>
       <c r="B50" s="2" t="s">
         <v>70</v>
       </c>
@@ -2267,10 +2269,10 @@
       <c r="E50" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F50" s="10"/>
+      <c r="F50" s="4"/>
     </row>
     <row r="51" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A51" s="5"/>
+      <c r="A51" s="11"/>
       <c r="B51" s="2" t="s">
         <v>50</v>
       </c>
@@ -2278,15 +2280,15 @@
         <v>19</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F51" s="10"/>
+      <c r="F51" s="4"/>
     </row>
     <row r="52" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A52" s="5"/>
+      <c r="A52" s="11"/>
       <c r="B52" s="2" t="s">
         <v>51</v>
       </c>
@@ -2294,15 +2296,15 @@
         <v>35</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F52" s="10"/>
+      <c r="F52" s="4"/>
     </row>
     <row r="53" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A53" s="5"/>
+      <c r="A53" s="11"/>
       <c r="B53" s="2" t="s">
         <v>52</v>
       </c>
@@ -2310,15 +2312,15 @@
         <v>18</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F53" s="10"/>
+      <c r="F53" s="4"/>
     </row>
     <row r="54" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A54" s="5"/>
+      <c r="A54" s="11"/>
       <c r="B54" s="2" t="s">
         <v>53</v>
       </c>
@@ -2326,15 +2328,15 @@
         <v>19</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F54" s="10"/>
+      <c r="F54" s="4"/>
     </row>
     <row r="55" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A55" s="9"/>
+      <c r="A55" s="12"/>
       <c r="B55" s="2" t="s">
         <v>12</v>
       </c>
@@ -2342,15 +2344,15 @@
         <v>19</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F55" s="10"/>
+      <c r="F55" s="4"/>
     </row>
     <row r="56" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="10" t="s">
         <v>63</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -2360,15 +2362,15 @@
         <v>13</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F56" s="10"/>
+      <c r="F56" s="4"/>
     </row>
     <row r="57" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A57" s="5"/>
+      <c r="A57" s="11"/>
       <c r="B57" s="2" t="s">
         <v>49</v>
       </c>
@@ -2376,15 +2378,15 @@
         <v>19</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F57" s="10"/>
+      <c r="F57" s="4"/>
     </row>
     <row r="58" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A58" s="5"/>
+      <c r="A58" s="11"/>
       <c r="B58" s="2" t="s">
         <v>69</v>
       </c>
@@ -2397,10 +2399,10 @@
       <c r="E58" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F58" s="10"/>
+      <c r="F58" s="4"/>
     </row>
     <row r="59" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A59" s="5"/>
+      <c r="A59" s="11"/>
       <c r="B59" s="2" t="s">
         <v>70</v>
       </c>
@@ -2413,10 +2415,10 @@
       <c r="E59" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F59" s="10"/>
+      <c r="F59" s="4"/>
     </row>
     <row r="60" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A60" s="5"/>
+      <c r="A60" s="11"/>
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
@@ -2424,15 +2426,15 @@
         <v>15</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F60" s="10"/>
+      <c r="F60" s="4"/>
     </row>
     <row r="61" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A61" s="5"/>
+      <c r="A61" s="11"/>
       <c r="B61" s="2" t="s">
         <v>10</v>
       </c>
@@ -2445,10 +2447,10 @@
       <c r="E61" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F61" s="10"/>
+      <c r="F61" s="4"/>
     </row>
     <row r="62" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A62" s="5"/>
+      <c r="A62" s="11"/>
       <c r="B62" s="2" t="s">
         <v>55</v>
       </c>
@@ -2456,15 +2458,15 @@
         <v>35</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F62" s="10"/>
+      <c r="F62" s="4"/>
     </row>
     <row r="63" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A63" s="5"/>
+      <c r="A63" s="11"/>
       <c r="B63" s="2" t="s">
         <v>56</v>
       </c>
@@ -2472,15 +2474,15 @@
         <v>35</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F63" s="10"/>
+      <c r="F63" s="4"/>
     </row>
     <row r="64" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A64" s="5"/>
+      <c r="A64" s="11"/>
       <c r="B64" s="2" t="s">
         <v>57</v>
       </c>
@@ -2488,15 +2490,15 @@
         <v>64</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F64" s="10"/>
+      <c r="F64" s="4"/>
     </row>
     <row r="65" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A65" s="5"/>
+      <c r="A65" s="11"/>
       <c r="B65" s="2" t="s">
         <v>58</v>
       </c>
@@ -2504,15 +2506,15 @@
         <v>64</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F65" s="10"/>
+      <c r="F65" s="4"/>
     </row>
     <row r="66" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A66" s="5"/>
+      <c r="A66" s="11"/>
       <c r="B66" s="2" t="s">
         <v>59</v>
       </c>
@@ -2520,15 +2522,15 @@
         <v>35</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F66" s="10"/>
+      <c r="F66" s="4"/>
     </row>
     <row r="67" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A67" s="5"/>
+      <c r="A67" s="11"/>
       <c r="B67" s="2" t="s">
         <v>60</v>
       </c>
@@ -2536,15 +2538,15 @@
         <v>35</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F67" s="10"/>
+      <c r="F67" s="4"/>
     </row>
     <row r="68" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A68" s="5"/>
+      <c r="A68" s="11"/>
       <c r="B68" s="2" t="s">
         <v>61</v>
       </c>
@@ -2552,15 +2554,15 @@
         <v>18</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F68" s="10"/>
+      <c r="F68" s="4"/>
     </row>
     <row r="69" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A69" s="5"/>
+      <c r="A69" s="11"/>
       <c r="B69" s="2" t="s">
         <v>62</v>
       </c>
@@ -2568,15 +2570,15 @@
         <v>19</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F69" s="10"/>
+      <c r="F69" s="4"/>
     </row>
     <row r="70" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A70" s="5"/>
+      <c r="A70" s="11"/>
       <c r="B70" s="2" t="s">
         <v>12</v>
       </c>
@@ -2584,15 +2586,15 @@
         <v>19</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F70" s="10"/>
+      <c r="F70" s="4"/>
     </row>
     <row r="71" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A71" s="12" t="s">
+      <c r="A71" s="6" t="s">
         <v>67</v>
       </c>
       <c r="B71" s="2" t="s">
@@ -2602,15 +2604,15 @@
         <v>13</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F71" s="10"/>
+      <c r="F71" s="4"/>
     </row>
     <row r="72" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A72" s="12"/>
+      <c r="A72" s="6"/>
       <c r="B72" s="2" t="s">
         <v>69</v>
       </c>
@@ -2623,10 +2625,10 @@
       <c r="E72" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F72" s="10"/>
+      <c r="F72" s="4"/>
     </row>
     <row r="73" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A73" s="12"/>
+      <c r="A73" s="6"/>
       <c r="B73" s="2" t="s">
         <v>70</v>
       </c>
@@ -2639,10 +2641,10 @@
       <c r="E73" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F73" s="10"/>
+      <c r="F73" s="4"/>
     </row>
     <row r="74" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A74" s="12"/>
+      <c r="A74" s="6"/>
       <c r="B74" s="2" t="s">
         <v>6</v>
       </c>
@@ -2650,15 +2652,15 @@
         <v>15</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F74" s="10"/>
+      <c r="F74" s="4"/>
     </row>
     <row r="75" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A75" s="12"/>
+      <c r="A75" s="6"/>
       <c r="B75" s="2" t="s">
         <v>49</v>
       </c>
@@ -2666,15 +2668,15 @@
         <v>19</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F75" s="10"/>
+      <c r="F75" s="4"/>
     </row>
     <row r="76" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A76" s="12"/>
+      <c r="A76" s="6"/>
       <c r="B76" s="2" t="s">
         <v>55</v>
       </c>
@@ -2682,15 +2684,15 @@
         <v>35</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F76" s="10"/>
+      <c r="F76" s="4"/>
     </row>
     <row r="77" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A77" s="12"/>
+      <c r="A77" s="6"/>
       <c r="B77" s="2" t="s">
         <v>65</v>
       </c>
@@ -2698,15 +2700,15 @@
         <v>64</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F77" s="10"/>
+      <c r="F77" s="4"/>
     </row>
     <row r="78" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A78" s="12"/>
+      <c r="A78" s="6"/>
       <c r="B78" s="2" t="s">
         <v>66</v>
       </c>
@@ -2714,15 +2716,15 @@
         <v>15</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F78" s="10"/>
+      <c r="F78" s="4"/>
     </row>
     <row r="79" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A79" s="12"/>
+      <c r="A79" s="6"/>
       <c r="B79" s="2" t="s">
         <v>12</v>
       </c>
@@ -2730,12 +2732,12 @@
         <v>19</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F79" s="10"/>
+      <c r="F79" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
COMPROBACION DATO A DATO PAGO UNICO EN FUNCIONES CORRECCION PIVOTES
</commit_message>
<xml_diff>
--- a/mapeo PU.xlsx
+++ b/mapeo PU.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ruchva\senasir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ruchva\code-dba-helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="195">
   <si>
     <t>Mapeo de datos origen y destino - PAGO UNICO</t>
   </si>
@@ -1287,6 +1287,135 @@
       </rPr>
       <t>TIPO_CAMBIO</t>
     </r>
+  </si>
+  <si>
+    <t>NUPAsegurado</t>
+  </si>
+  <si>
+    <t>IdBeneficioOtorgado</t>
+  </si>
+  <si>
+    <t>IdCampoAplicacion</t>
+  </si>
+  <si>
+    <t>FechaOtorgamiento</t>
+  </si>
+  <si>
+    <t>PeridoInicioPago</t>
+  </si>
+  <si>
+    <t>PeriodoFinalPago</t>
+  </si>
+  <si>
+    <t>IdEstadoBeneficio</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>FechaConclusionBeneficio</t>
+  </si>
+  <si>
+    <t>NroTramiteProceso</t>
+  </si>
+  <si>
+    <t>AplicaDescuento</t>
+  </si>
+  <si>
+    <t>IdTipoTramiteProceso</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>NUP de DocumentoComparativo</t>
+  </si>
+  <si>
+    <t>IdGrupoBeneficio de DocumentoComparativo</t>
+  </si>
+  <si>
+    <t>BeneficioAsegurado</t>
+  </si>
+  <si>
+    <t>IdTipoDocumento</t>
+  </si>
+  <si>
+    <t>IdEstadoCivil</t>
+  </si>
+  <si>
+    <t>IdEntidadGestora</t>
+  </si>
+  <si>
+    <t>IdSexo</t>
+  </si>
+  <si>
+    <t>CUA</t>
+  </si>
+  <si>
+    <t>Matricula</t>
+  </si>
+  <si>
+    <t>NUB</t>
+  </si>
+  <si>
+    <t>ComplementoSEGIP</t>
+  </si>
+  <si>
+    <t>IdDocumentoExpedido</t>
+  </si>
+  <si>
+    <t>PrimerNombre</t>
+  </si>
+  <si>
+    <t>SegundoNombre</t>
+  </si>
+  <si>
+    <t>PrimerApellido</t>
+  </si>
+  <si>
+    <t>SegundoApellido</t>
+  </si>
+  <si>
+    <t>ApellidoCasada</t>
+  </si>
+  <si>
+    <t>FechaNacimiento</t>
+  </si>
+  <si>
+    <t>FechaFallecimiento</t>
+  </si>
+  <si>
+    <t>IdPaisResidencia</t>
+  </si>
+  <si>
+    <t>CorreoElectronico</t>
+  </si>
+  <si>
+    <t>Celular</t>
+  </si>
+  <si>
+    <t>Direccion</t>
+  </si>
+  <si>
+    <t>IdLocalidad</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>IdHuella</t>
+  </si>
+  <si>
+    <t>FechaRegistroPersona</t>
+  </si>
+  <si>
+    <t>IdUsuarioRegistro</t>
+  </si>
+  <si>
+    <t>bigint identity</t>
+  </si>
+  <si>
+    <t>Persona</t>
   </si>
 </sst>
 </file>
@@ -1414,7 +1543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1454,6 +1583,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1736,16 +1874,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
@@ -3352,8 +3490,606 @@
       </c>
       <c r="F100" s="4"/>
     </row>
+    <row r="101" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A101" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F101" s="4"/>
+    </row>
+    <row r="102" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A102" s="9"/>
+      <c r="B102" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F102" s="4"/>
+    </row>
+    <row r="103" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A103" s="9"/>
+      <c r="B103" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D103" s="3"/>
+      <c r="E103" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F103" s="4"/>
+    </row>
+    <row r="104" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A104" s="9"/>
+      <c r="B104" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F104" s="4"/>
+    </row>
+    <row r="105" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A105" s="9"/>
+      <c r="B105" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F105" s="4"/>
+    </row>
+    <row r="106" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A106" s="9"/>
+      <c r="B106" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D106" s="2"/>
+      <c r="E106" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F106" s="4"/>
+    </row>
+    <row r="107" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A107" s="9"/>
+      <c r="B107" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F107" s="4"/>
+    </row>
+    <row r="108" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A108" s="9"/>
+      <c r="B108" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F108" s="4"/>
+    </row>
+    <row r="109" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A109" s="9"/>
+      <c r="B109" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D109" s="3"/>
+      <c r="E109" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F109" s="4"/>
+    </row>
+    <row r="110" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A110" s="9"/>
+      <c r="B110" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F110" s="4"/>
+    </row>
+    <row r="111" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A111" s="9"/>
+      <c r="B111" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F111" s="4"/>
+    </row>
+    <row r="112" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A112" s="9"/>
+      <c r="B112" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F112" s="4"/>
+    </row>
+    <row r="113" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A113" s="9"/>
+      <c r="B113" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F113" s="4"/>
+    </row>
+    <row r="114" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A114" s="9"/>
+      <c r="B114" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F114" s="4"/>
+    </row>
+    <row r="115" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A115" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D115" s="3"/>
+      <c r="E115" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F115" s="4"/>
+    </row>
+    <row r="116" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A116" s="18"/>
+      <c r="B116" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D116" s="3"/>
+      <c r="E116" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F116" s="4"/>
+    </row>
+    <row r="117" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A117" s="18"/>
+      <c r="B117" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D117" s="3"/>
+      <c r="E117" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F117" s="4"/>
+    </row>
+    <row r="118" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A118" s="18"/>
+      <c r="B118" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D118" s="2"/>
+      <c r="E118" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F118" s="4"/>
+    </row>
+    <row r="119" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A119" s="18"/>
+      <c r="B119" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F119" s="4"/>
+    </row>
+    <row r="120" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A120" s="18"/>
+      <c r="B120" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D120" s="2"/>
+      <c r="E120" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F120" s="4"/>
+    </row>
+    <row r="121" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A121" s="18"/>
+      <c r="B121" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D121" s="2"/>
+      <c r="E121" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F121" s="4"/>
+    </row>
+    <row r="122" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A122" s="18"/>
+      <c r="B122" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F122" s="4"/>
+    </row>
+    <row r="123" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A123" s="18"/>
+      <c r="B123" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D123" s="3"/>
+      <c r="E123" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F123" s="4"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="18"/>
+      <c r="B124" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D124" s="4"/>
+      <c r="E124" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F124" s="4"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="18"/>
+      <c r="B125" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D125" s="4"/>
+      <c r="E125" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F125" s="4"/>
+    </row>
+    <row r="126" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A126" s="18"/>
+      <c r="B126" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D126" s="3"/>
+      <c r="E126" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F126" s="4"/>
+    </row>
+    <row r="127" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A127" s="18"/>
+      <c r="B127" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D127" s="3"/>
+      <c r="E127" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F127" s="4"/>
+    </row>
+    <row r="128" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A128" s="18"/>
+      <c r="B128" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D128" s="3"/>
+      <c r="E128" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F128" s="4"/>
+    </row>
+    <row r="129" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A129" s="18"/>
+      <c r="B129" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D129" s="2"/>
+      <c r="E129" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F129" s="4"/>
+    </row>
+    <row r="130" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A130" s="18"/>
+      <c r="B130" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D130" s="2"/>
+      <c r="E130" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F130" s="4"/>
+    </row>
+    <row r="131" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A131" s="18"/>
+      <c r="B131" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D131" s="2"/>
+      <c r="E131" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F131" s="4"/>
+    </row>
+    <row r="132" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A132" s="18"/>
+      <c r="B132" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D132" s="2"/>
+      <c r="E132" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F132" s="4"/>
+    </row>
+    <row r="133" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A133" s="18"/>
+      <c r="B133" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D133" s="2"/>
+      <c r="E133" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F133" s="4"/>
+    </row>
+    <row r="134" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A134" s="18"/>
+      <c r="B134" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D134" s="3"/>
+      <c r="E134" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F134" s="4"/>
+    </row>
+    <row r="135" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A135" s="18"/>
+      <c r="B135" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D135" s="3"/>
+      <c r="E135" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F135" s="4"/>
+    </row>
+    <row r="136" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A136" s="18"/>
+      <c r="B136" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D136" s="3"/>
+      <c r="E136" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F136" s="4"/>
+    </row>
+    <row r="137" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A137" s="18"/>
+      <c r="B137" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D137" s="2"/>
+      <c r="E137" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F137" s="4"/>
+    </row>
+    <row r="138" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A138" s="18"/>
+      <c r="B138" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D138" s="2"/>
+      <c r="E138" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F138" s="4"/>
+    </row>
+    <row r="139" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A139" s="18"/>
+      <c r="B139" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D139" s="2"/>
+      <c r="E139" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F139" s="4"/>
+    </row>
+    <row r="140" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A140" s="18"/>
+      <c r="B140" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D140" s="2"/>
+      <c r="E140" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F140" s="4"/>
+    </row>
+    <row r="141" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A141" s="18"/>
+      <c r="B141" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D141" s="2"/>
+      <c r="E141" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F141" s="4"/>
+    </row>
+    <row r="142" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A142" s="19"/>
+      <c r="B142" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D142" s="3"/>
+      <c r="E142" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F142" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="A115:A142"/>
+    <mergeCell ref="A101:A114"/>
     <mergeCell ref="A92:A100"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A18:A31"/>

</xml_diff>